<commit_message>
move sjsdm code to the HJA_scripts folder
</commit_message>
<xml_diff>
--- a/HJA_scripts/08_reference_sequences_datasets/pa_vs_qp_tables_20201206.xlsx
+++ b/HJA_scripts/08_reference_sequences_datasets/pa_vs_qp_tables_20201206.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Negorashi2011/Dropbox/Working_docs/Luo_Mingjie_Oregon/qSeq paper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Negorashi2011/Dropbox/Working_docs/Luo_Mingjie_Oregon/HJA_analyses_Kelpie/HJA_scripts/08_reference_sequences_datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3B171D-5093-3245-9E01-4F19F013ED85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6401E214-E70D-C645-9DD7-4B2259E6C015}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{53C8B974-4F2E-7B4E-B4C5-DAE879BD5093}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
   <si>
     <t>OTU01</t>
   </si>
@@ -102,9 +102,6 @@
     <t>suboptimal env conditions</t>
   </si>
   <si>
-    <t>family=negative.binomial</t>
-  </si>
-  <si>
     <t>spikeOTU</t>
   </si>
   <si>
@@ -174,7 +171,16 @@
     <t>Compare Tables 2a and 1a. They are not alike, showing the effect of row noise</t>
   </si>
   <si>
-    <t>in mvabund, use offset(log(1/spikeOTU)) OR composition=TRUE</t>
+    <t>manyglm(otu.ord ~ 1, composition=TRUE, family="negative.binomial")</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>manyglm(otu.ord ~ 1 + offset(log(spikeOTU)), family="negative.binomial")</t>
+  </si>
+  <si>
+    <t>mvabund::</t>
   </si>
 </sst>
 </file>
@@ -467,6 +473,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -475,21 +496,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1710,7 +1716,7 @@
   <dimension ref="A1:Z46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S39" sqref="S39"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1746,24 +1752,24 @@
     <row r="2" spans="2:26" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
-      <c r="D2" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="54" t="s">
-        <v>35</v>
+      <c r="D2" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="50" t="s">
+        <v>34</v>
       </c>
       <c r="J2" s="53"/>
       <c r="K2" s="11"/>
-      <c r="Q2" s="55" t="s">
-        <v>21</v>
-      </c>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
+      <c r="Q2" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
       <c r="U2" s="28"/>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.2">
@@ -1782,9 +1788,9 @@
         <v>3</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="54"/>
+        <v>16</v>
+      </c>
+      <c r="I3" s="50"/>
       <c r="J3" s="53"/>
       <c r="K3" s="11"/>
       <c r="Q3" s="24" t="s">
@@ -1983,7 +1989,7 @@
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
       <c r="Q8" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.2">
@@ -2004,37 +2010,37 @@
       <c r="V10" s="11"/>
     </row>
     <row r="11" spans="2:26" s="5" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="56" t="s">
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="54" t="s">
-        <v>25</v>
-      </c>
-      <c r="L11" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="M11" s="52"/>
-      <c r="N11" s="52"/>
-      <c r="O11" s="52"/>
-      <c r="Q11" s="52" t="s">
+      <c r="J11" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="R11" s="52"/>
-      <c r="S11" s="52"/>
-      <c r="T11" s="52"/>
-      <c r="W11" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="X11" s="50"/>
-      <c r="Y11" s="50"/>
-      <c r="Z11" s="51"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
+      <c r="Q11" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="R11" s="49"/>
+      <c r="S11" s="49"/>
+      <c r="T11" s="49"/>
+      <c r="W11" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="X11" s="55"/>
+      <c r="Y11" s="55"/>
+      <c r="Z11" s="56"/>
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.2">
       <c r="D12" s="24" t="s">
@@ -2050,10 +2056,10 @@
         <v>3</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="56"/>
-      <c r="J12" s="54"/>
+        <v>16</v>
+      </c>
+      <c r="I12" s="52"/>
+      <c r="J12" s="50"/>
       <c r="L12" s="24" t="s">
         <v>0</v>
       </c>
@@ -2079,7 +2085,7 @@
         <v>3</v>
       </c>
       <c r="W12" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="X12" s="41"/>
       <c r="Y12" s="41"/>
@@ -2151,7 +2157,7 @@
         <v>0</v>
       </c>
       <c r="W13" s="43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="X13" s="41"/>
       <c r="Y13" s="41"/>
@@ -2255,7 +2261,7 @@
         <v>630</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L15" s="3">
         <f t="shared" si="3"/>
@@ -2413,11 +2419,11 @@
       <c r="Z17" s="42"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="K18" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="L18" t="s">
-        <v>40</v>
-      </c>
-      <c r="S18" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="W18" s="21"/>
       <c r="X18" s="6"/>
@@ -2428,8 +2434,11 @@
       <c r="F19" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L19" s="8" t="s">
-        <v>16</v>
+      <c r="K19" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="L19" t="s">
+        <v>39</v>
       </c>
       <c r="W19" s="44" t="s">
         <v>14</v>
@@ -2439,6 +2448,9 @@
       <c r="Z19" s="42"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="S20" t="s">
+        <v>7</v>
+      </c>
       <c r="W20" s="45" t="s">
         <v>15</v>
       </c>
@@ -2447,23 +2459,23 @@
       <c r="Z20" s="42"/>
     </row>
     <row r="21" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D21" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="52"/>
-      <c r="Q21" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="R21" s="52"/>
-      <c r="S21" s="52"/>
-      <c r="T21" s="52"/>
-      <c r="U21" s="54" t="s">
-        <v>36</v>
+      <c r="D21" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="Q21" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="R21" s="49"/>
+      <c r="S21" s="49"/>
+      <c r="T21" s="49"/>
+      <c r="U21" s="50" t="s">
+        <v>35</v>
       </c>
       <c r="W21" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="X21" s="6"/>
       <c r="Y21" s="6"/>
@@ -2494,9 +2506,9 @@
       <c r="T22" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="U22" s="54"/>
+      <c r="U22" s="50"/>
       <c r="W22" s="43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X22" s="6"/>
       <c r="Y22" s="6"/>
@@ -2706,7 +2718,7 @@
       <c r="B27" s="8"/>
       <c r="C27" s="11"/>
       <c r="D27" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
@@ -2720,14 +2732,14 @@
       <c r="N27" s="8"/>
       <c r="O27" s="8"/>
       <c r="Q27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B28" s="8"/>
       <c r="C28" s="11"/>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
@@ -2756,12 +2768,12 @@
     <row r="30" spans="1:26" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="8"/>
       <c r="C30" s="11"/>
-      <c r="D30" s="52" t="s">
-        <v>34</v>
-      </c>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
+      <c r="D30" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
       <c r="J30" s="11"/>
@@ -2891,7 +2903,7 @@
     </row>
     <row r="36" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D36" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
@@ -2902,12 +2914,12 @@
       <c r="O36" s="11"/>
     </row>
     <row r="39" spans="4:15" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D39" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="E39" s="52"/>
-      <c r="F39" s="52"/>
-      <c r="G39" s="52"/>
+      <c r="D39" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="49"/>
     </row>
     <row r="40" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D40" s="24" t="s">
@@ -2981,7 +2993,7 @@
     </row>
     <row r="45" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D45" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
@@ -2989,18 +3001,11 @@
     </row>
     <row r="46" spans="4:15" x14ac:dyDescent="0.2">
       <c r="D46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J2:J3"/>
     <mergeCell ref="W11:Z11"/>
     <mergeCell ref="D39:G39"/>
     <mergeCell ref="L11:O11"/>
@@ -3010,6 +3015,13 @@
     <mergeCell ref="Q21:T21"/>
     <mergeCell ref="Q11:T11"/>
     <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="J2:J3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>